<commit_message>
added new samples (thanks joseph)
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFC4E84-275B-4286-BD7F-7339FC715011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D459A81-D755-47ED-9284-70A5DEB17C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11970" yWindow="750" windowWidth="17745" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="61">
   <si>
     <t>id</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>msg</t>
+  </si>
+  <si>
+    <t>click to accept a packet</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,6 +1431,35 @@
         <v>57</v>
       </c>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1">
+        <v>44380</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding 3 more samples
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D459A81-D755-47ED-9284-70A5DEB17C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B87F9FE-105E-4BEF-B7D4-DC8962B8CA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="63">
   <si>
     <t>id</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>click to accept a packet</t>
+  </si>
+  <si>
+    <t>click to see mature content</t>
+  </si>
+  <si>
+    <t>click to confirm delivery</t>
   </si>
 </sst>
 </file>
@@ -527,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,6 +1466,93 @@
         <v>60</v>
       </c>
     </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="1">
+        <v>44380</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44380</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="1">
+        <v>44380</v>
+      </c>
+      <c r="D32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding entity column to dataset
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B87F9FE-105E-4BEF-B7D4-DC8962B8CA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CB1065-C6B1-45CB-B9AA-7986AF872608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -141,9 +141,6 @@
     <t>2facode</t>
   </si>
   <si>
-    <t>request for 2facode</t>
-  </si>
-  <si>
     <t>https://www.centralbankmalta.org/phishing-attempt-2021</t>
   </si>
   <si>
@@ -214,6 +211,57 @@
   </si>
   <si>
     <t>click to confirm delivery</t>
+  </si>
+  <si>
+    <t>request for 2fa code</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>DHL</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>HSBC</t>
+  </si>
+  <si>
+    <t>MaltaPost</t>
+  </si>
+  <si>
+    <t>BOV,HSBC</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>BOV</t>
+  </si>
+  <si>
+    <t>CentralBank</t>
+  </si>
+  <si>
+    <t>Melita</t>
+  </si>
+  <si>
+    <t>MTA</t>
+  </si>
+  <si>
+    <t>ChinaUniversity</t>
+  </si>
+  <si>
+    <t>LIDL</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>MeDirect</t>
   </si>
 </sst>
 </file>
@@ -533,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,10 +598,11 @@
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="105.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="105.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,15 +631,18 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1">
         <v>44363</v>
@@ -614,15 +666,18 @@
         <v>21</v>
       </c>
       <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1">
         <v>44363</v>
@@ -646,15 +701,18 @@
         <v>21</v>
       </c>
       <c r="J3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1">
         <v>44364</v>
@@ -678,10 +736,13 @@
         <v>24</v>
       </c>
       <c r="J4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -709,13 +770,16 @@
       <c r="I5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1">
         <v>44376</v>
@@ -739,15 +803,18 @@
         <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="K6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1">
         <v>44379</v>
@@ -770,8 +837,11 @@
       <c r="I7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -799,11 +869,14 @@
       <c r="I8" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -831,11 +904,14 @@
       <c r="I9" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -863,16 +939,19 @@
       <c r="I10" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="1">
         <v>44379</v>
@@ -895,16 +974,19 @@
       <c r="I11" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1">
         <v>44379</v>
@@ -927,16 +1009,19 @@
       <c r="I12" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1">
         <v>44379</v>
@@ -959,16 +1044,19 @@
       <c r="I13" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1">
         <v>44379</v>
@@ -991,16 +1079,19 @@
       <c r="I14" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1">
         <v>44379</v>
@@ -1023,16 +1114,19 @@
       <c r="I15" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1">
         <v>44379</v>
@@ -1055,16 +1149,19 @@
       <c r="I16" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1">
         <v>44379</v>
@@ -1087,11 +1184,14 @@
       <c r="I17" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1120,15 +1220,18 @@
         <v>36</v>
       </c>
       <c r="J18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1">
         <v>44379</v>
@@ -1149,18 +1252,21 @@
         <v>12</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="J19" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1">
         <v>44379</v>
@@ -1181,13 +1287,16 @@
         <v>12</v>
       </c>
       <c r="I20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="K20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1204,27 +1313,30 @@
         <v>31</v>
       </c>
       <c r="F21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" t="s">
         <v>41</v>
       </c>
-      <c r="G21" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21" t="s">
         <v>42</v>
       </c>
-      <c r="J21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1">
         <v>44379</v>
@@ -1245,13 +1357,16 @@
         <v>12</v>
       </c>
       <c r="I22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="K22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1277,10 +1392,13 @@
         <v>12</v>
       </c>
       <c r="I23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="J23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1297,24 +1415,27 @@
         <v>31</v>
       </c>
       <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" t="s">
         <v>48</v>
       </c>
-      <c r="G24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1">
         <v>44379</v>
@@ -1326,7 +1447,7 @@
         <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
         <v>20</v>
@@ -1335,18 +1456,21 @@
         <v>12</v>
       </c>
       <c r="I25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="K25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="1">
         <v>44379</v>
@@ -1358,7 +1482,7 @@
         <v>17</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" t="s">
         <v>20</v>
@@ -1367,13 +1491,16 @@
         <v>12</v>
       </c>
       <c r="I26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" t="s">
+        <v>76</v>
+      </c>
+      <c r="K26" t="s">
         <v>52</v>
       </c>
-      <c r="J26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1399,18 +1526,21 @@
         <v>12</v>
       </c>
       <c r="I27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="K27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="1">
         <v>44380</v>
@@ -1431,18 +1561,21 @@
         <v>12</v>
       </c>
       <c r="I28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="K28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="1">
         <v>44380</v>
@@ -1463,15 +1596,18 @@
         <v>12</v>
       </c>
       <c r="I29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="J29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" s="1">
         <v>44380</v>
@@ -1483,7 +1619,7 @@
         <v>17</v>
       </c>
       <c r="F30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G30" t="s">
         <v>13</v>
@@ -1492,15 +1628,18 @@
         <v>12</v>
       </c>
       <c r="I30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="J30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1">
         <v>44380</v>
@@ -1521,15 +1660,18 @@
         <v>12</v>
       </c>
       <c r="I31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="J31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="1">
         <v>44380</v>
@@ -1550,7 +1692,10 @@
         <v>12</v>
       </c>
       <c r="I32" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="J32" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better information for case 12
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B58C03-389F-4607-83FF-0FD5181C24E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F3B658-7F35-4357-979B-5E2FEC498F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="83">
   <si>
     <t>id</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>lang</t>
+  </si>
+  <si>
+    <t>https://timesofmalta.com/articles/view/maltapost-warns-customers-about-text-message-scam.862923</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1070,7 @@
         <v>65</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new attempt, more samples
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F3B658-7F35-4357-979B-5E2FEC498F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92087810-8290-48D3-8E69-1974040F92F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$35</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="83">
   <si>
     <t>id</t>
   </si>
@@ -602,11 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,7 +1711,7 @@
         <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H32" t="s">
         <v>11</v>
@@ -1784,7 +1787,40 @@
         <v>62</v>
       </c>
     </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="1">
+        <v>44382</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:K35" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added 2 news cases
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92087810-8290-48D3-8E69-1974040F92F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392FD2AA-B205-4F79-9A34-87B5ED34BD96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10470" yWindow="-615" windowWidth="17745" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="84">
   <si>
     <t>id</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>https://timesofmalta.com/articles/view/maltapost-warns-customers-about-text-message-scam.862923</t>
+  </si>
+  <si>
+    <t>confirm address for postal delivery</t>
   </si>
 </sst>
 </file>
@@ -605,11 +608,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1819,6 +1822,70 @@
         <v>65</v>
       </c>
     </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="1">
+        <v>44383</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="1">
+        <v>44383</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" t="s">
+        <v>83</v>
+      </c>
+      <c r="J37" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K35" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
split medirect in 2, added transcripts
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392FD2AA-B205-4F79-9A34-87B5ED34BD96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B67511-F063-47B8-BDAD-1EACD5D71150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10470" yWindow="-615" windowWidth="17745" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17745" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="85">
   <si>
     <t>id</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>confirm address for postal delivery</t>
+  </si>
+  <si>
+    <t>number changed, report if not recognised</t>
   </si>
 </sst>
 </file>
@@ -608,11 +611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,7 +1583,7 @@
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="G28" t="s">
         <v>18</v>
@@ -1726,7 +1729,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1884,6 +1887,41 @@
       </c>
       <c r="J37" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="1">
+        <v>44384</v>
+      </c>
+      <c r="D38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" t="s">
+        <v>84</v>
+      </c>
+      <c r="J38" t="s">
+        <v>76</v>
+      </c>
+      <c r="K38" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new sample, transcripts added, cleanup
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B67511-F063-47B8-BDAD-1EACD5D71150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0266510-822B-4DDC-9A57-1052C20E00C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17745" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$39</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="85">
   <si>
     <t>id</t>
   </si>
@@ -611,11 +611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1897,7 @@
         <v>56</v>
       </c>
       <c r="C38" s="1">
-        <v>44384</v>
+        <v>44383</v>
       </c>
       <c r="D38" t="s">
         <v>24</v>
@@ -1924,8 +1924,40 @@
         <v>53</v>
       </c>
     </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="1">
+        <v>44384</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K35" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new case + transcript fix
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6486F8C2-01B2-4361-8B18-FEF11B3136E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC222C8F-C9BD-426E-9FC5-36B5AAB8CE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="92">
   <si>
     <t>id</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>failed delivery to to missed payment</t>
+  </si>
+  <si>
+    <t>busines opportunity</t>
+  </si>
+  <si>
+    <t>Lombard</t>
   </si>
 </sst>
 </file>
@@ -627,11 +633,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,6 +2109,38 @@
         <v>65</v>
       </c>
     </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44384</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" t="s">
+        <v>45</v>
+      </c>
+      <c r="G44" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" t="s">
+        <v>11</v>
+      </c>
+      <c r="I44" t="s">
+        <v>90</v>
+      </c>
+      <c r="J44" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K42" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">

</xml_diff>

<commit_message>
added a case with 2 variants
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\github\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE220177-E7FD-4B4B-ACA6-0F0F850E3815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8428BFDA-78C3-487E-A578-2F822F4E27C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="94">
   <si>
     <t>id</t>
   </si>
@@ -638,29 +638,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="130.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7265625" customWidth="1"/>
+    <col min="11" max="11" width="130.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -695,7 +695,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -730,7 +730,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -765,7 +765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -800,7 +800,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -832,7 +832,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -902,7 +902,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -937,7 +937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -972,7 +972,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2147,6 +2147,38 @@
       </c>
       <c r="K44" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44416</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" t="s">
+        <v>83</v>
+      </c>
+      <c r="J45" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding new case, text only no msg pic
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\github\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8428BFDA-78C3-487E-A578-2F822F4E27C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE3B1C4-6E75-45BD-8879-3F8EFA0D127F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="97">
   <si>
     <t>id</t>
   </si>
@@ -310,6 +310,15 @@
   </si>
   <si>
     <t>https://timesofmalta.com/articles/view/parcel-delivery-scammers-targeting-people-with-personalised-messages.882985</t>
+  </si>
+  <si>
+    <t>GO,Melita</t>
+  </si>
+  <si>
+    <t>refund from telecoms</t>
+  </si>
+  <si>
+    <t>redirects to https://doctorbrew.pl/wp-admin/user/-/</t>
   </si>
 </sst>
 </file>
@@ -638,11 +647,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -883,9 +892,6 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
@@ -2179,6 +2185,41 @@
       </c>
       <c r="J45" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44416</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" t="s">
+        <v>95</v>
+      </c>
+      <c r="J46" t="s">
+        <v>94</v>
+      </c>
+      <c r="K46" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
splitting an attempt in 2 due to differences
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\github\malta-phishing-samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE3B1C4-6E75-45BD-8879-3F8EFA0D127F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75C5ED2-7EDC-4F74-A435-EEDE63A5E7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="98">
   <si>
     <t>id</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>redirects to https://doctorbrew.pl/wp-admin/user/-/</t>
+  </si>
+  <si>
+    <t>click to accept a packet, proper maltese fonts</t>
   </si>
 </sst>
 </file>
@@ -647,29 +650,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7265625" customWidth="1"/>
-    <col min="11" max="11" width="130.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="130.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -704,7 +707,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -739,7 +742,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -774,7 +777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -809,7 +812,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -841,7 +844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -876,7 +879,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -908,7 +911,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -943,7 +946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -978,7 +981,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1083,7 +1086,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1188,7 +1191,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1223,7 +1226,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1433,7 +1436,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1567,7 +1570,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1829,7 +1832,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1893,7 +1896,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1960,7 +1963,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1992,7 +1995,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2056,7 +2059,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2088,7 +2091,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2120,7 +2123,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2155,7 +2158,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2220,6 +2223,38 @@
       </c>
       <c r="K46" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="1">
+        <v>44416</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" t="s">
+        <v>97</v>
+      </c>
+      <c r="J47" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2 new attempts, one new variant
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75C5ED2-7EDC-4F74-A435-EEDE63A5E7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45963EA-CC83-4EBA-8CD6-559B82F9FDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="101">
   <si>
     <t>id</t>
   </si>
@@ -322,12 +322,24 @@
   </si>
   <si>
     <t>click to accept a packet, proper maltese fonts</t>
+  </si>
+  <si>
+    <t>get a free covid kit</t>
+  </si>
+  <si>
+    <t>redirects to https://www.restaurant-apron.at/wp-admin/network/-/</t>
+  </si>
+  <si>
+    <t>delivery payment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -367,9 +379,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,11 +662,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,38 +684,38 @@
     <col min="11" max="11" width="130.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>78</v>
       </c>
     </row>
@@ -714,7 +726,7 @@
       <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>44363</v>
       </c>
       <c r="D2" t="s">
@@ -749,7 +761,7 @@
       <c r="B3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>44363</v>
       </c>
       <c r="D3" t="s">
@@ -784,7 +796,7 @@
       <c r="B4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>44364</v>
       </c>
       <c r="D4" t="s">
@@ -819,7 +831,7 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>44368</v>
       </c>
       <c r="D5" t="s">
@@ -851,7 +863,7 @@
       <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>44376</v>
       </c>
       <c r="D6" t="s">
@@ -886,7 +898,7 @@
       <c r="B7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>44379</v>
       </c>
       <c r="D7" t="s">
@@ -918,7 +930,7 @@
       <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>44379</v>
       </c>
       <c r="D8" t="s">
@@ -942,7 +954,7 @@
       <c r="J8" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -953,7 +965,7 @@
       <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>44379</v>
       </c>
       <c r="D9" t="s">
@@ -977,7 +989,7 @@
       <c r="J9" t="s">
         <v>65</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -988,7 +1000,7 @@
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>44379</v>
       </c>
       <c r="D10" t="s">
@@ -1012,7 +1024,7 @@
       <c r="J10" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1023,7 +1035,7 @@
       <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>44379</v>
       </c>
       <c r="D11" t="s">
@@ -1047,7 +1059,7 @@
       <c r="J11" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1058,7 +1070,7 @@
       <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>44379</v>
       </c>
       <c r="D12" t="s">
@@ -1082,7 +1094,7 @@
       <c r="J12" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1093,7 +1105,7 @@
       <c r="B13" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>44379</v>
       </c>
       <c r="D13" t="s">
@@ -1117,7 +1129,7 @@
       <c r="J13" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1128,7 +1140,7 @@
       <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>44379</v>
       </c>
       <c r="D14" t="s">
@@ -1152,7 +1164,7 @@
       <c r="J14" t="s">
         <v>65</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1163,7 +1175,7 @@
       <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <v>44379</v>
       </c>
       <c r="D15" t="s">
@@ -1187,7 +1199,7 @@
       <c r="J15" t="s">
         <v>65</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1198,7 +1210,7 @@
       <c r="B16" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>44379</v>
       </c>
       <c r="D16" t="s">
@@ -1222,7 +1234,7 @@
       <c r="J16" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1233,7 +1245,7 @@
       <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>44379</v>
       </c>
       <c r="D17" t="s">
@@ -1257,7 +1269,7 @@
       <c r="J17" t="s">
         <v>63</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1268,7 +1280,7 @@
       <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
         <v>44379</v>
       </c>
       <c r="D18" t="s">
@@ -1303,7 +1315,7 @@
       <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="3">
         <v>44379</v>
       </c>
       <c r="D19" t="s">
@@ -1338,7 +1350,7 @@
       <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>44379</v>
       </c>
       <c r="D20" t="s">
@@ -1373,7 +1385,7 @@
       <c r="B21" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="3">
         <v>44379</v>
       </c>
       <c r="D21" t="s">
@@ -1408,7 +1420,7 @@
       <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="3">
         <v>44379</v>
       </c>
       <c r="D22" t="s">
@@ -1443,7 +1455,7 @@
       <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="3">
         <v>44379</v>
       </c>
       <c r="D23" t="s">
@@ -1475,7 +1487,7 @@
       <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="3">
         <v>44379</v>
       </c>
       <c r="D24" t="s">
@@ -1507,7 +1519,7 @@
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="3">
         <v>44379</v>
       </c>
       <c r="D25" t="s">
@@ -1542,7 +1554,7 @@
       <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="3">
         <v>44379</v>
       </c>
       <c r="D26" t="s">
@@ -1577,7 +1589,7 @@
       <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="3">
         <v>44379</v>
       </c>
       <c r="D27" t="s">
@@ -1612,7 +1624,7 @@
       <c r="B28" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="3">
         <v>44380</v>
       </c>
       <c r="D28" t="s">
@@ -1647,7 +1659,7 @@
       <c r="B29" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="3">
         <v>44380</v>
       </c>
       <c r="D29" t="s">
@@ -1679,7 +1691,7 @@
       <c r="B30" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="3">
         <v>44380</v>
       </c>
       <c r="D30" t="s">
@@ -1711,7 +1723,7 @@
       <c r="B31" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="3">
         <v>44380</v>
       </c>
       <c r="D31" t="s">
@@ -1743,7 +1755,7 @@
       <c r="B32" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="3">
         <v>44380</v>
       </c>
       <c r="D32" t="s">
@@ -1775,7 +1787,7 @@
       <c r="B33" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="3">
         <v>44380</v>
       </c>
       <c r="D33" t="s">
@@ -1807,7 +1819,7 @@
       <c r="B34" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="3">
         <v>44380</v>
       </c>
       <c r="D34" t="s">
@@ -1839,7 +1851,7 @@
       <c r="B35" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="3">
         <v>44382</v>
       </c>
       <c r="D35" t="s">
@@ -1871,7 +1883,7 @@
       <c r="B36" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="3">
         <v>44383</v>
       </c>
       <c r="D36" t="s">
@@ -1903,7 +1915,7 @@
       <c r="B37" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="3">
         <v>44383</v>
       </c>
       <c r="D37" t="s">
@@ -1935,7 +1947,7 @@
       <c r="B38" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="3">
         <v>44383</v>
       </c>
       <c r="D38" t="s">
@@ -1970,7 +1982,7 @@
       <c r="B39" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="3">
         <v>44384</v>
       </c>
       <c r="D39" t="s">
@@ -2002,7 +2014,7 @@
       <c r="B40" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="3">
         <v>44384</v>
       </c>
       <c r="D40" t="s">
@@ -2034,7 +2046,7 @@
       <c r="B41" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="3">
         <v>44384</v>
       </c>
       <c r="D41" t="s">
@@ -2066,7 +2078,7 @@
       <c r="B42" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="3">
         <v>44384</v>
       </c>
       <c r="D42" t="s">
@@ -2098,7 +2110,7 @@
       <c r="B43" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="3">
         <v>44384</v>
       </c>
       <c r="D43" t="s">
@@ -2130,7 +2142,7 @@
       <c r="B44" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="3">
         <v>44384</v>
       </c>
       <c r="D44" t="s">
@@ -2165,8 +2177,8 @@
       <c r="B45" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="1">
-        <v>44416</v>
+      <c r="C45" s="3">
+        <v>44385</v>
       </c>
       <c r="D45" t="s">
         <v>16</v>
@@ -2197,8 +2209,8 @@
       <c r="B46" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="1">
-        <v>44416</v>
+      <c r="C46" s="3">
+        <v>44385</v>
       </c>
       <c r="D46" t="s">
         <v>16</v>
@@ -2227,13 +2239,13 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="1">
-        <v>44416</v>
+      <c r="C47" s="3">
+        <v>44385</v>
       </c>
       <c r="D47" t="s">
         <v>16</v>
@@ -2255,6 +2267,73 @@
       </c>
       <c r="J47" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="3">
+        <v>44389</v>
+      </c>
+      <c r="D48" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" t="s">
+        <v>45</v>
+      </c>
+      <c r="G48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" t="s">
+        <v>98</v>
+      </c>
+      <c r="J48" t="s">
+        <v>67</v>
+      </c>
+      <c r="K48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="3">
+        <v>44389</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" t="s">
+        <v>100</v>
+      </c>
+      <c r="J49" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a new attempt targeted at mcast
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45963EA-CC83-4EBA-8CD6-559B82F9FDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3A0216-4E10-4869-80E2-386A87C6270B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="104">
   <si>
     <t>id</t>
   </si>
@@ -331,6 +331,15 @@
   </si>
   <si>
     <t>delivery payment</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>Verify to avoid lockout</t>
+  </si>
+  <si>
+    <t>redirects to https://officehotmail2021.weebly.com/</t>
   </si>
 </sst>
 </file>
@@ -338,7 +347,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -377,11 +386,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,11 +672,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,7 +2314,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2334,6 +2344,41 @@
       </c>
       <c r="J49" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="4">
+        <v>44390</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" t="s">
+        <v>102</v>
+      </c>
+      <c r="J50" t="s">
+        <v>16</v>
+      </c>
+      <c r="K50" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new covid case, new column
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\github\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A8674B-F094-44F9-A4A4-D84D8BE9A304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC06848-A367-4613-BD59-10CDCF44FFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="114">
   <si>
     <t>id</t>
   </si>
@@ -318,18 +318,12 @@
     <t>refund from telecoms</t>
   </si>
   <si>
-    <t>redirects to https://doctorbrew.pl/wp-admin/user/-/</t>
-  </si>
-  <si>
     <t>click to accept a packet, proper maltese fonts</t>
   </si>
   <si>
     <t>get a free covid kit</t>
   </si>
   <si>
-    <t>redirects to https://www.restaurant-apron.at/wp-admin/network/-/</t>
-  </si>
-  <si>
     <t>delivery payment</t>
   </si>
   <si>
@@ -339,12 +333,6 @@
     <t>Verify to avoid lockout</t>
   </si>
   <si>
-    <t>redirects to https://officehotmail2021.weebly.com/</t>
-  </si>
-  <si>
-    <t>redirects to https://watson.pe/onlineBov/</t>
-  </si>
-  <si>
     <t>Account reset</t>
   </si>
   <si>
@@ -358,6 +346,30 @@
   </si>
   <si>
     <t>https://timesofmalta.com/articles/view/customs-department-warns-people-about-email-scam.887101</t>
+  </si>
+  <si>
+    <t>buy covid passport</t>
+  </si>
+  <si>
+    <t>https://doctorbrew.pl/wp-admin/user/-/</t>
+  </si>
+  <si>
+    <t>https://www.restaurant-apron.at/wp-admin/network/-/</t>
+  </si>
+  <si>
+    <t>https://officehotmail2021.weebly.com/</t>
+  </si>
+  <si>
+    <t>https://watson.pe/onlineBov/</t>
+  </si>
+  <si>
+    <t>https://dhl-mt-cliint-srvscs-soynius-rfiid-delivery-sophiechappot211321.codeanyapp.com/mtxx/index1.php</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/story.php?story_fbid=4377523138997877&amp;id=488536334563263</t>
+  </si>
+  <si>
+    <t>redirectsto</t>
   </si>
 </sst>
 </file>
@@ -690,29 +702,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K55" sqref="K55"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="130.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7265625" customWidth="1"/>
+    <col min="11" max="11" width="122.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="91.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -746,8 +761,11 @@
       <c r="K1" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -782,7 +800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -817,7 +835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -852,7 +870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -884,7 +902,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -919,7 +937,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -951,7 +969,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -986,7 +1004,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1021,7 +1039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1056,7 +1074,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1091,7 +1109,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1126,7 +1144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1161,7 +1179,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1196,7 +1214,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1231,7 +1249,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1266,7 +1284,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1301,7 +1319,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1336,7 +1354,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1371,7 +1389,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1406,7 +1424,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1441,7 +1459,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1476,7 +1494,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1508,7 +1526,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1540,7 +1558,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1575,7 +1593,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1610,7 +1628,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1645,7 +1663,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1680,7 +1698,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1712,7 +1730,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1744,7 +1762,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1776,7 +1794,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1808,7 +1826,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1840,7 +1858,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1872,7 +1890,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1904,7 +1922,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1936,7 +1954,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1968,7 +1986,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2003,7 +2021,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2035,7 +2053,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2067,7 +2085,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2099,7 +2117,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2131,7 +2149,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2163,7 +2181,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2198,7 +2216,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2230,7 +2248,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2261,11 +2279,11 @@
       <c r="J46" t="s">
         <v>94</v>
       </c>
-      <c r="K46" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2291,13 +2309,13 @@
         <v>11</v>
       </c>
       <c r="I47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J47" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2323,16 +2341,16 @@
         <v>11</v>
       </c>
       <c r="I48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J48" t="s">
         <v>67</v>
       </c>
-      <c r="K48" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2358,18 +2376,18 @@
         <v>11</v>
       </c>
       <c r="I49" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J49" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C50" s="4">
         <v>44390</v>
@@ -2390,16 +2408,16 @@
         <v>11</v>
       </c>
       <c r="I50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J50" t="s">
         <v>16</v>
       </c>
-      <c r="K50" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2425,16 +2443,16 @@
         <v>11</v>
       </c>
       <c r="I51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J51" t="s">
         <v>68</v>
       </c>
-      <c r="K51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2460,13 +2478,13 @@
         <v>11</v>
       </c>
       <c r="I52" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J52" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2492,13 +2510,13 @@
         <v>11</v>
       </c>
       <c r="I53" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J53" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2524,13 +2542,51 @@
         <v>11</v>
       </c>
       <c r="I54" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J54" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K54" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="4">
+        <v>44408</v>
+      </c>
+      <c r="D55" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" t="s">
+        <v>106</v>
+      </c>
+      <c r="J55" t="s">
+        <v>67</v>
+      </c>
+      <c r="K55" t="s">
+        <v>112</v>
+      </c>
+      <c r="L55" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new covid kit variant
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\mcast\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61723F2-BB1D-4BDC-9B20-0D845BCB43E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF76D56-70EE-438D-8458-3A4CC0038210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="121">
   <si>
     <t>id</t>
   </si>
@@ -364,10 +364,6 @@
   </si>
   <si>
     <t>redirectsto</t>
-  </si>
-  <si>
-    <t>https://www.restaurant-apron.at/wp-admin/network/-/
-https://certifikatvaccin-gov-mt-sophiechappot211321.codeanyapp.com/mtxx/</t>
   </si>
   <si>
     <t>https://trackingmalta.pro/BOV/bov/bov/</t>
@@ -391,6 +387,14 @@
   <si>
     <t>https://dhl-mt-cliint-srvscs-soynius-rfiid-delivery-sophiechappot211321.codeanyapp.com/mtxx/index1.php
 https://certifikatvaccin-gov-residents-ofmaltaonly-yakuzablyat101350359.codeanyapp.com/online/</t>
+  </si>
+  <si>
+    <t>https://www.restaurant-apron.at/wp-admin/network/-/
+https://certifikatvaccin-gov-mt-sophiechappot211321.codeanyapp.com/mtxx/
+https://www.autorepar.com.br/wp-admin/images/--/</t>
+  </si>
+  <si>
+    <t>https://www.tvm.com.mt/en/news/watch-out-for-deceitful-message-about-covid-19/</t>
   </si>
 </sst>
 </file>
@@ -729,10 +733,10 @@
   <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L56" sqref="L56"/>
+      <selection pane="bottomRight" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1277,7 @@
         <v>27</v>
       </c>
       <c r="L15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1853,7 +1857,7 @@
         <v>68</v>
       </c>
       <c r="L32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2345,7 +2349,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2376,8 +2380,11 @@
       <c r="J48" t="s">
         <v>67</v>
       </c>
+      <c r="K48" t="s">
+        <v>120</v>
+      </c>
       <c r="L48" s="5" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2616,7 +2623,7 @@
         <v>110</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2636,7 +2643,7 @@
         <v>14</v>
       </c>
       <c r="F56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G56" t="s">
         <v>12</v>
@@ -2645,13 +2652,13 @@
         <v>11</v>
       </c>
       <c r="I56" t="s">
+        <v>115</v>
+      </c>
+      <c r="J56" t="s">
         <v>116</v>
       </c>
-      <c r="J56" t="s">
+      <c r="K56" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
variants of  known cases
</commit_message>
<xml_diff>
--- a/samples-details.xlsx
+++ b/samples-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\github\malta-phishing-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0666EFF-C041-4128-958B-78B2FBDDD451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161FC11B-31EE-44A8-9BF2-CECE46ACEBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,15 +390,16 @@
 https://www.autorepar.com.br/wp-admin/images/--/</t>
   </si>
   <si>
-    <t>https://www.tvm.com.mt/en/news/watch-out-for-deceitful-message-about-covid-19/</t>
-  </si>
-  <si>
     <t>click to claim win</t>
   </si>
   <si>
     <t>https://dhl-mt-cliint-srvscs-soynius-rfiid-delivery-sophiechappot211321.codeanyapp.com/mtxx/index1.php
 https://certifikatvaccin-gov-residents-ofmaltaonly-yakuzablyat101350359.codeanyapp.com/online/
 https://zelfstandigeadviseurs.nl/wp-content/themes/twentytwentyone/-/</t>
+  </si>
+  <si>
+    <t>https://www.tvm.com.mt/en/news/watch-out-for-deceitful-message-about-covid-19/
+https://www.facebook.com/101043071614245/posts/389400936111789/</t>
   </si>
 </sst>
 </file>
@@ -737,10 +738,10 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L56" sqref="L56"/>
+      <selection pane="bottomRight" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2364,7 +2365,7 @@
         <v>44389</v>
       </c>
       <c r="D48" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
@@ -2384,8 +2385,8 @@
       <c r="J48" t="s">
         <v>67</v>
       </c>
-      <c r="K48" t="s">
-        <v>119</v>
+      <c r="K48" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>118</v>
@@ -2627,7 +2628,7 @@
         <v>110</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -2723,7 +2724,7 @@
         <v>31</v>
       </c>
       <c r="I58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J58" t="s">
         <v>73</v>

</xml_diff>